<commit_message>
Made tables for main text
</commit_message>
<xml_diff>
--- a/Figures_Tables/Q1_Q2_Q3_Data_transformations.xlsx
+++ b/Figures_Tables/Q1_Q2_Q3_Data_transformations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_one\Figures_Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0854EBA-6113-47D1-A070-FA5F633050FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36211A23-7271-462C-9C21-0EEE835F8776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80262A53-80DF-4B6A-BAE3-37A7C27E9108}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{80262A53-80DF-4B6A-BAE3-37A7C27E9108}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Transformations" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="39">
   <si>
     <t>Trait</t>
   </si>
@@ -183,12 +183,28 @@
   <si>
     <t>Species Evenness</t>
   </si>
+  <si>
+    <t>log(1-x)</t>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>³</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +296,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -319,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -812,11 +833,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -838,22 +874,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,9 +981,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -970,9 +991,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1005,159 +1023,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1170,27 +1035,186 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1509,672 +1533,722 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04ADC99-E54C-4A00-9468-470DAE17135C}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="40" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.77734375" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="7" style="40" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="40"/>
-    <col min="12" max="12" width="18.109375" style="40" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" style="40" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" style="40" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="40"/>
+    <col min="1" max="1" width="12.5546875" style="36" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="7" style="36" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="36"/>
+    <col min="12" max="12" width="18.109375" style="36" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" style="36" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" style="36" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="L1" s="86" t="s">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="L1" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="96" t="s">
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="97"/>
-      <c r="N2" s="90" t="s">
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="116"/>
+      <c r="N2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="91"/>
-      <c r="P2" s="90" t="s">
+      <c r="O2" s="88"/>
+      <c r="P2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="91"/>
+      <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99" t="s">
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="100"/>
-      <c r="N3" s="101" t="s">
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="119"/>
+      <c r="N3" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="102"/>
-      <c r="P3" s="101" t="s">
+      <c r="O3" s="90"/>
+      <c r="P3" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="102"/>
+      <c r="Q3" s="90"/>
     </row>
     <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="44" t="s">
+      <c r="J4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="42" t="s">
+      <c r="M4" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="N4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="46" t="s">
+      <c r="P4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="49" t="s">
+      <c r="D5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="94" t="s">
+      <c r="H5" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="52" t="s">
+      <c r="M5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="O5" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="54"/>
+      <c r="N5" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="50" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="108"/>
-      <c r="B6" s="55" t="s">
+      <c r="A6" s="96"/>
+      <c r="B6" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="56" t="s">
+      <c r="D6" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="95"/>
-      <c r="M6" s="59" t="s">
+      <c r="H6" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="114"/>
+      <c r="M6" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="61"/>
+      <c r="N6" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="57" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="107" t="s">
+      <c r="C7" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="66" t="s">
+      <c r="M7" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="49" t="s">
+      <c r="N7" s="141" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="68"/>
+      <c r="O7" s="142" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="142" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="93"/>
-      <c r="B8" s="69" t="s">
+      <c r="A8" s="112"/>
+      <c r="B8" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="108"/>
-      <c r="M8" s="55" t="s">
+      <c r="C8" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="96"/>
+      <c r="M8" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="49" t="s">
+      <c r="N8" s="141" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="74"/>
+      <c r="O8" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="141" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="68" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="105" t="s">
+      <c r="A9" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="56" t="s">
+      <c r="D9" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="78" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="56" t="s">
+      <c r="H9" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="142" t="s">
+      <c r="L9" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="143" t="s">
+      <c r="M9" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="141" t="s">
+      <c r="N9" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="146" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="147"/>
-      <c r="Q9" s="146"/>
+      <c r="O9" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="143" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="86" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="106"/>
-      <c r="B10" s="79" t="s">
+      <c r="A10" s="94"/>
+      <c r="B10" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="80" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="56" t="s">
+      <c r="D10" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="80" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="56" t="s">
+      <c r="H10" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="144"/>
-      <c r="M10" s="145" t="s">
+      <c r="L10" s="102"/>
+      <c r="M10" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="141" t="s">
-        <v>31</v>
-      </c>
-      <c r="O10" s="148" t="s">
-        <v>10</v>
-      </c>
-      <c r="P10" s="149"/>
-      <c r="Q10" s="148"/>
+      <c r="N10" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" s="81" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="115" t="s">
+      <c r="C11" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23"/>
+      <c r="N11" s="140" t="s">
+        <v>16</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="140" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="112"/>
-      <c r="B12" s="69" t="s">
+      <c r="A12" s="100"/>
+      <c r="B12" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="116"/>
+      <c r="C12" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="104"/>
       <c r="M12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="25"/>
+      <c r="N12" s="144" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" s="144" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="125" t="s">
+      <c r="C13" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="105" t="s">
         <v>36</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="139" t="s">
-        <v>16</v>
-      </c>
-      <c r="O13" s="137" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="19"/>
+      <c r="N13" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13" s="80" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="110"/>
-      <c r="B14" s="55" t="s">
+      <c r="A14" s="98"/>
+      <c r="B14" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="126"/>
+      <c r="C14" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="106"/>
       <c r="M14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="141" t="s">
+      <c r="N14" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="O14" s="138" t="s">
-        <v>10</v>
-      </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
+      <c r="O14" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14" s="81" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="84"/>
+      <c r="K16" s="78"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="104" t="s">
+      <c r="A17" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="84"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="104"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="92"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="104"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
+      <c r="E19" s="92"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="104"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="104"/>
-      <c r="K20" s="84"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="92"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="K20" s="78"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="104"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
-      <c r="K21" s="85"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="K21" s="79"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="103"/>
+      <c r="B22" s="91"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="36" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="36" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A22:G22"/>
@@ -2187,16 +2261,6 @@
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2207,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC2DC81-BE91-4B65-9D19-3394C309B6B2}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:Q14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,77 +2286,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="133" t="s">
+      <c r="L1" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
-      <c r="O1" s="133"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="124"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="133"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="119" t="s">
+      <c r="N2" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="121"/>
+      <c r="O2" s="129"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="130"/>
     </row>
     <row r="3" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135" t="s">
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="136"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="123"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="113" t="s">
+      <c r="N3" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="114"/>
-      <c r="P3" s="113" t="s">
+      <c r="O3" s="125"/>
+      <c r="P3" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="114"/>
+      <c r="Q3" s="125"/>
     </row>
     <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -2346,38 +2410,38 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="103" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="26" t="s">
+      <c r="C5" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="26" t="s">
+      <c r="G5" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="22" t="s">
         <v>28</v>
       </c>
       <c r="K5" s="5"/>
-      <c r="L5" s="125" t="s">
+      <c r="L5" s="105" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="7" t="s">
@@ -2386,422 +2450,457 @@
       <c r="N5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="137" t="s">
+      <c r="O5" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="19"/>
+      <c r="P5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="80" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="116"/>
+      <c r="A6" s="104"/>
       <c r="B6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="26" t="s">
+      <c r="C6" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="26" t="s">
+      <c r="G6" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="22" t="s">
         <v>28</v>
       </c>
       <c r="K6" s="5"/>
-      <c r="L6" s="126"/>
+      <c r="L6" s="106"/>
       <c r="M6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="O6" s="138" t="s">
+      <c r="N6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="21"/>
+      <c r="P6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="81" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="127" t="s">
+      <c r="A7" s="134" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="32" t="s">
+      <c r="C7" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="32" t="s">
+      <c r="G7" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="28" t="s">
         <v>29</v>
       </c>
       <c r="K7" s="5"/>
-      <c r="L7" s="115" t="s">
+      <c r="L7" s="103" t="s">
         <v>20</v>
       </c>
       <c r="M7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="23"/>
+      <c r="N7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="128"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="32" t="s">
+      <c r="C8" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="32" t="s">
+      <c r="G8" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="28" t="s">
         <v>29</v>
       </c>
       <c r="K8" s="5"/>
-      <c r="L8" s="116"/>
+      <c r="L8" s="104"/>
       <c r="M8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="25"/>
+      <c r="N8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="129" t="s">
+      <c r="A9" s="136" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="26" t="s">
+      <c r="C9" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="26" t="s">
+      <c r="G9" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="22" t="s">
         <v>28</v>
       </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="127" t="s">
+      <c r="L9" s="134" t="s">
         <v>34</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="139" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="137" t="s">
-        <v>10</v>
-      </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="19"/>
+      <c r="N9" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="80" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="130"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="26" t="s">
+      <c r="C10" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="26" t="s">
+      <c r="G10" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="22" t="s">
         <v>28</v>
       </c>
       <c r="K10" s="5"/>
-      <c r="L10" s="128"/>
+      <c r="L10" s="135"/>
       <c r="M10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="140" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" s="138" t="s">
-        <v>10</v>
-      </c>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="21"/>
+      <c r="N10" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="P10" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="81" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="131" t="s">
+      <c r="A11" s="138" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="30" t="s">
+      <c r="C11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="26" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="115" t="s">
+      <c r="L11" s="103" t="s">
         <v>35</v>
       </c>
       <c r="M11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23"/>
+      <c r="N11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="132"/>
+      <c r="A12" s="139"/>
       <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="33" t="s">
+      <c r="C12" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="29" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="5"/>
-      <c r="L12" s="116"/>
+      <c r="L12" s="104"/>
       <c r="M12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="O12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="25"/>
+      <c r="N12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="126" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="26" t="s">
+      <c r="C13" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="22" t="s">
         <v>10</v>
       </c>
       <c r="K13" s="5"/>
-      <c r="L13" s="125" t="s">
+      <c r="L13" s="105" t="s">
         <v>36</v>
       </c>
       <c r="M13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="139" t="s">
-        <v>30</v>
-      </c>
-      <c r="O13" s="137" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="19"/>
+      <c r="N13" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="80" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="118"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="28" t="s">
+      <c r="C14" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="24" t="s">
         <v>10</v>
       </c>
       <c r="K14" s="5"/>
-      <c r="L14" s="126"/>
+      <c r="L14" s="106"/>
       <c r="M14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="140" t="s">
-        <v>30</v>
-      </c>
-      <c r="O14" s="138" t="s">
-        <v>10</v>
-      </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
+      <c r="N14" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="81" t="s">
+        <v>10</v>
+      </c>
+      <c r="P14" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="81" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="A13:A14"/>
@@ -2815,6 +2914,11 @@
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L13:L14"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>